<commit_message>
Stage 2. Created connections between new appended nodes and graph. Part 3. Need tests
</commit_message>
<xml_diff>
--- a/loader/src/main/resources/CropRegion_new1.xlsx
+++ b/loader/src/main/resources/CropRegion_new1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23802"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BD6C77A-AED0-48FC-BB47-0099DF85BD80}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80B8B79E-1D8A-475A-8AE3-8420278E8B5A}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,15 +105,15 @@
     <t>new-crop-description-id-2</t>
   </si>
   <si>
-    <t>new-country-id-2</t>
-  </si>
-  <si>
     <t>new-yield-base-unit-id-2</t>
   </si>
   <si>
     <t>new-demand-base-unit-id-2</t>
   </si>
   <si>
+    <t>new-region-id-2</t>
+  </si>
+  <si>
     <t>New crop description 2</t>
   </si>
   <si>
@@ -123,7 +123,7 @@
     <t>new-crop-description-id-3</t>
   </si>
   <si>
-    <t>new-country-id-3</t>
+    <t>8ca9994b-cfda-4699-9381-61c1f801ac97</t>
   </si>
   <si>
     <t>new-yield-base-unit-id-3</t>
@@ -132,7 +132,7 @@
     <t>new-demand-base-unit-id-3</t>
   </si>
   <si>
-    <t>c4bb0ddf-3a8d-4c0c-8643-fa39c8819a1f</t>
+    <t>eb290e84-1d10-472e-aa66-50d554362aea</t>
   </si>
   <si>
     <t>New crop description 3</t>
@@ -201,13 +201,13 @@
     <t>new-crop-description-id-8</t>
   </si>
   <si>
-    <t>b4260501-534a-4a00-a9de-0900e6169f1f</t>
+    <t>eb8759f4-a9a8-4b79-ba24-2538cc8fc4d6</t>
   </si>
   <si>
     <t>964672a4-01b8-46d3-9d80-dcbf66ecb937</t>
   </si>
   <si>
-    <t>e7bdceec-fe83-4d9a-ac6c-fa4348bd3a64</t>
+    <t>425cb4fc-c662-42cb-b59e-0ef61b159cac</t>
   </si>
   <si>
     <t>New crop description 8</t>
@@ -225,7 +225,7 @@
     <t>74255580-9feb-4fc2-a5ee-7635a4161bbf</t>
   </si>
   <si>
-    <t>fce9da03-03b4-4a7f-921c-55e7f0315b55</t>
+    <t>08dfead4-392e-4fe6-8966-505e6f16d7a4</t>
   </si>
   <si>
     <t>New crop description 9</t>
@@ -604,27 +604,11 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:J10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5703125" customWidth="1"/>
-    <col min="12" max="12" width="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="103.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="1" t="s">
@@ -716,7 +700,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -731,13 +715,13 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
       </c>
       <c r="K3" t="s">
         <v>18</v>
@@ -830,7 +814,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>43</v>
@@ -851,7 +835,7 @@
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
         <v>18</v>
@@ -883,10 +867,10 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
         <v>26</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>

</xml_diff>